<commit_message>
Atualização de código e revisão de resultados
</commit_message>
<xml_diff>
--- a/Face recognition/face recognition-resultados.xlsx
+++ b/Face recognition/face recognition-resultados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\isilon-l3\Perfil-l3\thais\Documents\TCC-master\Face recognition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsuba\Desktop\TCC-master\Face recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48AE0C5-CB00-4C8F-9CC6-194168C20455}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resultado-face_recognition-2" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'resultado-face_recognition-2'!$A$1:$F$2641</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss.0"/>
@@ -996,6 +997,33 @@
     <xf numFmtId="47" fontId="13" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1014,47 +1042,20 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1087,10 +1088,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1376,7 +1377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K2641"/>
   <sheetViews>
@@ -54228,7 +54229,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F2641">
+  <autoFilter ref="A1:F2641" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="1"/>
@@ -54246,7 +54247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -54269,40 +54270,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="42" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="42" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="42" t="s">
+      <c r="H1" s="52"/>
+      <c r="I1" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="43"/>
-      <c r="K1" s="40" t="s">
+      <c r="J1" s="52"/>
+      <c r="K1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="57"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="32" t="s">
         <v>13</v>
       </c>
@@ -54327,18 +54328,18 @@
       <c r="J2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="39" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="58">
+      <c r="B3" s="47">
         <f>SUM(C3,G3,I3)</f>
         <v>7</v>
       </c>
@@ -54369,11 +54370,11 @@
       <c r="K3" s="21">
         <v>1.3657407407407409E-3</v>
       </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -55125,7 +55126,7 @@
       <c r="A25" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="55">
+      <c r="B25" s="46">
         <f>SUM(B3:B24)</f>
         <v>120</v>
       </c>
@@ -55185,7 +55186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -55195,206 +55196,206 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="46">
-        <v>2</v>
-      </c>
-      <c r="B2" s="47">
+      <c r="A2" s="56">
+        <v>2</v>
+      </c>
+      <c r="B2" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49">
+      <c r="A3" s="58"/>
+      <c r="B3" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51">
+      <c r="A4" s="57"/>
+      <c r="B4" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="46">
-        <v>3</v>
-      </c>
-      <c r="B5" s="47">
+      <c r="A5" s="56">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51">
+      <c r="A6" s="57"/>
+      <c r="B6" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52">
+      <c r="A7" s="43">
         <v>5</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="52">
-        <v>6</v>
-      </c>
-      <c r="B8" s="53">
+      <c r="A8" s="43">
+        <v>6</v>
+      </c>
+      <c r="B8" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52">
-        <v>8</v>
-      </c>
-      <c r="B9" s="53">
+      <c r="A9" s="43">
+        <v>8</v>
+      </c>
+      <c r="B9" s="44">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52">
+      <c r="A10" s="43">
         <v>9</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="44">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52">
+      <c r="A11" s="43">
         <v>10</v>
       </c>
-      <c r="B11" s="53">
+      <c r="B11" s="44">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52">
+      <c r="A12" s="43">
         <v>12</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52">
+      <c r="A13" s="43">
         <v>13</v>
       </c>
-      <c r="B13" s="53">
+      <c r="B13" s="44">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52">
+      <c r="A14" s="43">
         <v>14</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B14" s="44">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="46">
+      <c r="A15" s="56">
         <v>15</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51">
+      <c r="A16" s="57"/>
+      <c r="B16" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="46">
+      <c r="A17" s="56">
         <v>16</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="40">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51">
+      <c r="A18" s="57"/>
+      <c r="B18" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="46">
+      <c r="A19" s="56">
         <v>17</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="40">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49">
+      <c r="A20" s="58"/>
+      <c r="B20" s="41">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51">
+      <c r="A21" s="57"/>
+      <c r="B21" s="42">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="46">
+      <c r="A22" s="56">
         <v>18</v>
       </c>
-      <c r="B22" s="47">
+      <c r="B22" s="40">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51">
+      <c r="A23" s="57"/>
+      <c r="B23" s="42">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
+      <c r="A24" s="56">
         <v>20</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B24" s="40">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51">
+      <c r="A25" s="57"/>
+      <c r="B25" s="42">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="46">
+      <c r="A26" s="56">
         <v>21</v>
       </c>
-      <c r="B26" s="47">
+      <c r="B26" s="40">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51">
+      <c r="A27" s="57"/>
+      <c r="B27" s="42">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="54">
+      <c r="B28" s="45">
         <f>COUNT(B2:B27)</f>
         <v>26</v>
       </c>

</xml_diff>